<commit_message>
Rapport et tableaux finaux (en tout cas on espère \o/)
</commit_message>
<xml_diff>
--- a/synthese/tableaux.xlsx
+++ b/synthese/tableaux.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Glouton" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="52">
   <si>
     <t>EcartType</t>
   </si>
@@ -127,9 +127,6 @@
     <t>It/sec</t>
   </si>
   <si>
-    <t>-1.#IND</t>
-  </si>
-  <si>
     <t>Exemplaire</t>
   </si>
   <si>
@@ -158,6 +155,27 @@
   </si>
   <si>
     <t>EA</t>
+  </si>
+  <si>
+    <t>18.1</t>
+  </si>
+  <si>
+    <t>25.4</t>
+  </si>
+  <si>
+    <t>40.5</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>107.1</t>
+  </si>
+  <si>
+    <t>133.7</t>
+  </si>
+  <si>
+    <t>1.26886</t>
   </si>
 </sst>
 </file>
@@ -255,11 +273,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1440,8 +1458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,7 +1552,7 @@
       <c r="E3" s="6">
         <v>22</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>200</v>
       </c>
       <c r="G3" s="6">
@@ -1574,7 +1592,7 @@
         <v>315158</v>
       </c>
       <c r="H4" s="7">
-        <f t="shared" ref="H3:H6" si="0">G4/F4</f>
+        <f t="shared" ref="H4:H6" si="0">G4/F4</f>
         <v>1575.79</v>
       </c>
       <c r="I4" s="6">
@@ -1660,8 +1678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,27 +1733,27 @@
       <c r="C2" s="8">
         <v>18</v>
       </c>
-      <c r="D2" s="8">
-        <v>18</v>
+      <c r="D2" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="E2" s="8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="8">
         <v>200</v>
       </c>
       <c r="G2" s="8">
-        <v>5186.22</v>
+        <v>33033.199999999997</v>
       </c>
       <c r="H2" s="8">
         <f>G2/F2</f>
-        <v>25.931100000000001</v>
-      </c>
-      <c r="I2" s="8">
-        <v>0</v>
+        <v>165.166</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="J2" s="8">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1746,29 +1764,29 @@
         <v>60</v>
       </c>
       <c r="C3" s="8">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E3" s="8">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="8" t="e">
+        <v>27</v>
+      </c>
+      <c r="F3" s="8">
+        <v>200</v>
+      </c>
+      <c r="G3" s="8">
+        <v>3821.9</v>
+      </c>
+      <c r="H3" s="8">
         <f t="shared" ref="H3:H6" si="0">G3/F3</f>
-        <v>#VALUE!</v>
+        <v>19.109500000000001</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="J3" s="8">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1781,27 +1799,27 @@
       <c r="C4" s="8">
         <v>40</v>
       </c>
-      <c r="D4" s="8">
-        <v>40</v>
+      <c r="D4" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="E4" s="8">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F4" s="8">
         <v>200</v>
       </c>
       <c r="G4" s="8">
-        <v>5707.5</v>
+        <v>35597.300000000003</v>
       </c>
       <c r="H4" s="8">
         <f t="shared" si="0"/>
-        <v>28.537500000000001</v>
-      </c>
-      <c r="I4" s="8">
-        <v>0</v>
+        <v>177.98650000000001</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="J4" s="8">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1812,29 +1830,29 @@
         <v>10</v>
       </c>
       <c r="C5" s="8">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="8" t="e">
+        <v>108</v>
+      </c>
+      <c r="F5" s="8">
+        <v>500</v>
+      </c>
+      <c r="G5" s="8">
+        <v>25226.1</v>
+      </c>
+      <c r="H5" s="8">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>50.452199999999998</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="J5" s="8">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1845,29 +1863,29 @@
         <v>15</v>
       </c>
       <c r="C6" s="8">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="8" t="e">
+        <v>136</v>
+      </c>
+      <c r="F6" s="8">
+        <v>500</v>
+      </c>
+      <c r="G6" s="8">
+        <v>11731.7</v>
+      </c>
+      <c r="H6" s="8">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>23.4634</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="J6" s="8">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1890,35 +1908,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="A1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="12"/>
+      <c r="J1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="12"/>
+      <c r="L1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="12"/>
+      <c r="N1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" s="11"/>
+      <c r="O1" s="12"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1928,43 +1946,43 @@
         <v>26</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="F2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="H2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="J2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="L2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="N2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>